<commit_message>
Agregar sismo a excel(Falta hacerlo bonito)
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -14,58 +14,58 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>Código</t>
+    <t>Fecha</t>
   </si>
   <si>
-    <t>Producto</t>
+    <t>Hora</t>
   </si>
   <si>
-    <t>Descripción</t>
+    <t>Profundidad</t>
   </si>
   <si>
-    <t>C001</t>
+    <t>Origen</t>
   </si>
   <si>
-    <t>SIRVIO</t>
+    <t>Detalle</t>
   </si>
   <si>
-    <t>Compurtador marca HP color negro.</t>
+    <t>Magnitud</t>
   </si>
   <si>
-    <t>C002</t>
+    <t>Latitud</t>
   </si>
   <si>
-    <t>Computador Escritorio Lenovo.</t>
+    <t>Longitud</t>
   </si>
   <si>
-    <t>Compurtador marca lenovo color negro con monitor integrado.</t>
+    <t>Provincia y descripcion Detallada</t>
   </si>
   <si>
-    <t>C003</t>
+    <t>Fri Jan 24 00:02:00 CST 2020</t>
   </si>
   <si>
-    <t>Impresora HP.</t>
+    <t>Thu Jan 01 10:10:10 CST 1970</t>
   </si>
   <si>
-    <t>Impresora marca HP, multifuncional color negro.</t>
+    <t>78.0</t>
   </si>
   <si>
-    <t>C004</t>
+    <t>SUBDUCCION_PLACA</t>
   </si>
   <si>
-    <t>Mouse Inalambrico Logitec.</t>
+    <t>hola</t>
   </si>
   <si>
-    <t>Mouse Inalambrico color azul con negro.</t>
+    <t>7.0</t>
   </si>
   <si>
-    <t>C005</t>
+    <t>8.0</t>
   </si>
   <si>
-    <t>Teclado Inalambrico Lenovo.</t>
+    <t>5.0</t>
   </si>
   <si>
-    <t>Teclado Inalambrico color blanco.</t>
+    <t>SAN_JOSE, nose</t>
   </si>
 </sst>
 </file>
@@ -116,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -132,59 +132,51 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregar sismo a JPanel(pero no leido del excel)
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -41,31 +41,31 @@
     <t>Provincia y descripcion Detallada</t>
   </si>
   <si>
-    <t>Fri Jan 24 00:02:00 CST 2020</t>
+    <t>24/02/2020</t>
   </si>
   <si>
-    <t>Thu Jan 01 10:10:10 CST 1970</t>
+    <t>02:02:20</t>
   </si>
   <si>
-    <t>78.0</t>
+    <t>7.0</t>
   </si>
   <si>
     <t>SUBDUCCION_PLACA</t>
   </si>
   <si>
-    <t>hola</t>
+    <t>nose</t>
   </si>
   <si>
-    <t>7.0</t>
+    <t>9.0</t>
   </si>
   <si>
-    <t>8.0</t>
+    <t>10.0</t>
   </si>
   <si>
     <t>5.0</t>
   </si>
   <si>
-    <t>SAN_JOSE, nose</t>
+    <t>SAN_JOSE, sirveee</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Metodo CrearExcel(No agrega mas de uno)
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Fecha</t>
   </si>
@@ -44,28 +44,25 @@
     <t>24/02/2020</t>
   </si>
   <si>
-    <t>02:02:20</t>
+    <t>02:02:08</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>SUBDUCCION_PLACA</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
   <si>
     <t>7.0</t>
   </si>
   <si>
-    <t>SUBDUCCION_PLACA</t>
-  </si>
-  <si>
-    <t>nose</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>SAN_JOSE, sirveee</t>
+    <t>SAN_JOSE, adios</t>
   </si>
 </sst>
 </file>
@@ -174,10 +171,10 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado lo del excel :100:
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Fecha</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>SAN_JOSE, adios</t>
+  </si>
+  <si>
+    <t>SIN_ASIGNAR, adios</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -177,6 +180,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Avance de Cargar( )
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -69,6 +69,36 @@
   </si>
   <si>
     <t>LIMON, adios</t>
+  </si>
+  <si>
+    <t>CHOQUE_PLACAS</t>
+  </si>
+  <si>
+    <t>HEREDIA, adios</t>
+  </si>
+  <si>
+    <t>24/02/2021</t>
+  </si>
+  <si>
+    <t>ALAJUELA, adios</t>
+  </si>
+  <si>
+    <t>24/02/2040</t>
+  </si>
+  <si>
+    <t>02:02:50</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>holo</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>PUNTARENAS, hola</t>
   </si>
 </sst>
 </file>
@@ -119,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -241,6 +271,151 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Validacion de Cajas texto
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1 SEMESTRE 2020\POO\PROYECTOS\Proyecto-1-de-POO-2020\Proyecto1_Sistema_Sismico\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E060507B-D688-4683-B85A-E78743E94767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" r:id="rId3" sheetId="1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
   <si>
     <t>Fecha</t>
   </si>
@@ -65,53 +73,53 @@
     <t>SAN_JOSE</t>
   </si>
   <si>
-    <t>CHOQUE_PLACAS</t>
-  </si>
-  <si>
-    <t>CARTAGO</t>
-  </si>
-  <si>
-    <t>24/12/2020</t>
-  </si>
-  <si>
-    <t>02:02:10</t>
-  </si>
-  <si>
-    <t>DEFORMACION_INTERNA</t>
-  </si>
-  <si>
-    <t>ALAJUELA</t>
-  </si>
-  <si>
-    <t>19/02/2020</t>
-  </si>
-  <si>
-    <t>24/15/2020</t>
-  </si>
-  <si>
-    <t>24/50/2020</t>
-  </si>
-  <si>
-    <t>24/01/2020</t>
+    <t>30/15/2020</t>
+  </si>
+  <si>
+    <t>29/00/2020</t>
+  </si>
+  <si>
+    <t>24/00/2025</t>
+  </si>
+  <si>
+    <t>24/00/2020</t>
+  </si>
+  <si>
+    <t>23:50:06</t>
+  </si>
+  <si>
+    <t>24/00/20200</t>
+  </si>
+  <si>
+    <t>02:03:25</t>
+  </si>
+  <si>
+    <t>78.0</t>
+  </si>
+  <si>
+    <t>23/00/2020</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,7 +127,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -136,20 +144,330 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -181,7 +499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -215,7 +533,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -247,7 +565,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -256,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -271,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
@@ -282,13 +600,13 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -303,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
@@ -311,7 +629,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -343,10 +661,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -375,10 +693,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -407,37 +725,133 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Algo que no da error
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="42">
   <si>
     <t>Fecha</t>
   </si>
@@ -504,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -553,7 +553,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -562,7 +562,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -804,6 +804,102 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creacion de Excel BD
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="91">
   <si>
     <t>Fecha</t>
   </si>
@@ -269,6 +269,30 @@
   </si>
   <si>
     <t>24/03/2013</t>
+  </si>
+  <si>
+    <t>24/01/2016</t>
+  </si>
+  <si>
+    <t>05:02:45</t>
+  </si>
+  <si>
+    <t>4.55</t>
+  </si>
+  <si>
+    <t>24/12/2016</t>
+  </si>
+  <si>
+    <t>89.8</t>
+  </si>
+  <si>
+    <t>67.2</t>
+  </si>
+  <si>
+    <t>Natalia</t>
+  </si>
+  <si>
+    <t>Sucedió</t>
   </si>
 </sst>
 </file>
@@ -627,7 +651,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -704,7 +728,7 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1441,6 +1465,134 @@
       </c>
       <c r="J25" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglo de CLase de excel
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="107">
   <si>
     <t>Fecha</t>
   </si>
@@ -293,6 +293,54 @@
   </si>
   <si>
     <t>Sucedió</t>
+  </si>
+  <si>
+    <t>24/07/2016</t>
+  </si>
+  <si>
+    <t>Probar si sirve</t>
+  </si>
+  <si>
+    <t>PUNTARENAS</t>
+  </si>
+  <si>
+    <t>cambio</t>
+  </si>
+  <si>
+    <t>HEREDIA</t>
+  </si>
+  <si>
+    <t>Hice un cambio</t>
+  </si>
+  <si>
+    <t>Hice cambio</t>
+  </si>
+  <si>
+    <t>cambiooo</t>
+  </si>
+  <si>
+    <t>nat</t>
+  </si>
+  <si>
+    <t>vanes</t>
+  </si>
+  <si>
+    <t>cambiossss</t>
+  </si>
+  <si>
+    <t>02:25:19</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ingrese los detalles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Más detalles</t>
+  </si>
+  <si>
+    <t>22:02:20</t>
   </si>
 </sst>
 </file>
@@ -651,7 +699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -701,66 +749,66 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -981,7 +1029,7 @@
         <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
         <v>44</v>
@@ -1365,7 +1413,7 @@
         <v>42</v>
       </c>
       <c r="I22" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="J22" t="s">
         <v>44</v>
@@ -1533,7 +1581,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
@@ -1560,7 +1608,7 @@
         <v>62</v>
       </c>
       <c r="J28" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29">
@@ -1593,6 +1641,134 @@
       </c>
       <c r="J29" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar sismos reales a la BD
</commit_message>
<xml_diff>
--- a/Proyecto1_Sistema_Sismico/BD.xlsx
+++ b/Proyecto1_Sistema_Sismico/BD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="181">
   <si>
     <t>Fecha</t>
   </si>
@@ -365,6 +365,204 @@
   </si>
   <si>
     <t>Se mejoro el mundo</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>Lugar poblado</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>9.906393</t>
+  </si>
+  <si>
+    <t>-83.67443</t>
+  </si>
+  <si>
+    <t>Peligroso</t>
+  </si>
+  <si>
+    <t>03/06/2020</t>
+  </si>
+  <si>
+    <t>23:55:17</t>
+  </si>
+  <si>
+    <t>Leve en Jacó</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>9.631</t>
+  </si>
+  <si>
+    <t>-84.7381</t>
+  </si>
+  <si>
+    <t>11.7 km oeste de Jacó,</t>
+  </si>
+  <si>
+    <t>01/06/2020</t>
+  </si>
+  <si>
+    <t>19:34:00</t>
+  </si>
+  <si>
+    <t>Leve en Turrialba centro</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>9.981</t>
+  </si>
+  <si>
+    <t>-83.71</t>
+  </si>
+  <si>
+    <t>8 km NO</t>
+  </si>
+  <si>
+    <t>26/04/2020</t>
+  </si>
+  <si>
+    <t>00:14:15</t>
+  </si>
+  <si>
+    <t>Reportado en: Puerto Carrillo, Punta Islita, Playa Sámara, Huacas, Hojancha, Nosara, Nicoya, Nandayure, Nambí, Filadelfia, Santa Cruz</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>9.8414</t>
+  </si>
+  <si>
+    <t>-85.5104</t>
+  </si>
+  <si>
+    <t>4.4 km Suroeste de Puerto Carrillo</t>
+  </si>
+  <si>
+    <t>20/04/2020</t>
+  </si>
+  <si>
+    <t>03:27:00</t>
+  </si>
+  <si>
+    <t>28.0</t>
+  </si>
+  <si>
+    <t>Reportado en :Talamanca, Valle de La Estrella y Limón</t>
+  </si>
+  <si>
+    <t>9.71</t>
+  </si>
+  <si>
+    <t>-82.8487</t>
+  </si>
+  <si>
+    <t>3 km al Suroeste de Cahuita</t>
+  </si>
+  <si>
+    <t>19/10/2019</t>
+  </si>
+  <si>
+    <t>07:06:56</t>
+  </si>
+  <si>
+    <t>45.7</t>
+  </si>
+  <si>
+    <t>Isla de Chira</t>
+  </si>
+  <si>
+    <t>4.41</t>
+  </si>
+  <si>
+    <t>10.0974</t>
+  </si>
+  <si>
+    <t>-85.1278</t>
+  </si>
+  <si>
+    <t>Marino</t>
+  </si>
+  <si>
+    <t>30/12/2017</t>
+  </si>
+  <si>
+    <t>07:38:00</t>
+  </si>
+  <si>
+    <t>9.33</t>
+  </si>
+  <si>
+    <t>-83.2865</t>
+  </si>
+  <si>
+    <t>17.4KM Noroeste</t>
+  </si>
+  <si>
+    <t>17:37:00</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>9.68</t>
+  </si>
+  <si>
+    <t>-84.87</t>
+  </si>
+  <si>
+    <t>17 Km Sede vaquera</t>
+  </si>
+  <si>
+    <t>28/12/2017</t>
+  </si>
+  <si>
+    <t>17:01:00</t>
+  </si>
+  <si>
+    <t>147.0</t>
+  </si>
+  <si>
+    <t>reportado en atena</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>15.5 km noroeste de Tilaran</t>
+  </si>
+  <si>
+    <t>10.6358</t>
+  </si>
+  <si>
+    <t>-84.7997</t>
+  </si>
+  <si>
+    <t>26/12/2017</t>
+  </si>
+  <si>
+    <t>17:20:00</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>9.46</t>
+  </si>
+  <si>
+    <t>-84.59</t>
+  </si>
+  <si>
+    <t>sureste de jaco</t>
   </si>
 </sst>
 </file>
@@ -723,7 +921,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -779,263 +977,263 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="J3" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1044,19 +1242,19 @@
         <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>178</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="I10" t="s">
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1117,7 +1315,7 @@
         <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="J12" t="s">
         <v>44</v>
@@ -1245,7 +1443,7 @@
         <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J16" t="s">
         <v>21</v>
@@ -1437,7 +1635,7 @@
         <v>42</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="J22" t="s">
         <v>44</v>
@@ -1469,7 +1667,7 @@
         <v>42</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="J23" t="s">
         <v>44</v>
@@ -1661,7 +1859,7 @@
         <v>16</v>
       </c>
       <c r="I29" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="J29" t="s">
         <v>89</v>
@@ -1725,7 +1923,7 @@
         <v>16</v>
       </c>
       <c r="I31" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="J31" t="s">
         <v>100</v>
@@ -1825,6 +2023,102 @@
       </c>
       <c r="J34" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" t="s">
+        <v>93</v>
+      </c>
+      <c r="J35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
+        <v>154</v>
+      </c>
+      <c r="H37" t="s">
+        <v>155</v>
+      </c>
+      <c r="I37" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>